<commit_message>
Alterações do nome de algumas variáveis e comentários novos.
</commit_message>
<xml_diff>
--- a/arq_backup/partidas.xlsx
+++ b/arq_backup/partidas.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leo\Desktop\trabalhoNovo\brasileirao\arq_backup\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -277,14 +277,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="135">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
+  <dxfs count="134">
     <dxf>
       <font>
         <b/>
@@ -1501,8 +1494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P380"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A240" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="E249" sqref="E249"/>
+    <sheetView tabSelected="1" topLeftCell="A215" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="J227" sqref="J227"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11623,7 +11616,7 @@
         <v>0</v>
       </c>
       <c r="D203" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E203" s="3" t="s">
         <v>6</v>
@@ -11635,7 +11628,7 @@
         <v>195</v>
       </c>
       <c r="H203" s="21">
-        <v>1000</v>
+        <v>195</v>
       </c>
       <c r="I203" s="21">
         <v>1000</v>
@@ -12770,10 +12763,10 @@
         <v>3</v>
       </c>
       <c r="C226" s="15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D226" s="25">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E226" s="5" t="s">
         <v>2</v>
@@ -12782,16 +12775,16 @@
         <v>12</v>
       </c>
       <c r="G226" s="21">
-        <v>1000</v>
+        <v>61</v>
       </c>
       <c r="H226" s="21">
-        <v>1000</v>
+        <v>61</v>
       </c>
       <c r="I226" s="21">
-        <v>1000</v>
+        <v>50</v>
       </c>
       <c r="J226" s="21">
-        <v>1000</v>
+        <v>50</v>
       </c>
       <c r="K226" s="21">
         <v>1000</v>
@@ -20514,662 +20507,672 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B380">
-    <cfRule type="cellIs" dxfId="134" priority="239" operator="equal">
+    <cfRule type="cellIs" dxfId="133" priority="241" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F380">
-    <cfRule type="cellIs" dxfId="133" priority="237" operator="equal">
+    <cfRule type="cellIs" dxfId="132" priority="239" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E380">
-    <cfRule type="cellIs" dxfId="132" priority="236" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="238" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:P1">
-    <cfRule type="cellIs" dxfId="131" priority="235" operator="equal">
+    <cfRule type="cellIs" dxfId="130" priority="237" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:J3">
-    <cfRule type="cellIs" dxfId="130" priority="234" operator="equal">
+    <cfRule type="cellIs" dxfId="129" priority="236" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G11:P20">
-    <cfRule type="cellIs" dxfId="129" priority="232" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="234" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G21:P30">
-    <cfRule type="cellIs" dxfId="128" priority="231" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="233" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G22:P30">
-    <cfRule type="cellIs" dxfId="127" priority="230" operator="equal">
+    <cfRule type="cellIs" dxfId="126" priority="232" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:K4">
-    <cfRule type="cellIs" dxfId="126" priority="176" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="178" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:J5">
-    <cfRule type="cellIs" dxfId="125" priority="175" operator="equal">
+    <cfRule type="cellIs" dxfId="124" priority="177" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:P2">
-    <cfRule type="cellIs" dxfId="124" priority="122" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="124" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:P3">
-    <cfRule type="cellIs" dxfId="123" priority="121" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="123" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4:P4">
-    <cfRule type="cellIs" dxfId="122" priority="120" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="122" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5:P5">
-    <cfRule type="cellIs" dxfId="121" priority="119" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="121" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6:P10">
-    <cfRule type="cellIs" dxfId="120" priority="118" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="120" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G31:P40">
-    <cfRule type="cellIs" dxfId="119" priority="117" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="119" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G41:P50">
-    <cfRule type="cellIs" dxfId="118" priority="116" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="118" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G42:P50">
-    <cfRule type="cellIs" dxfId="117" priority="115" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="117" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G51:P60">
-    <cfRule type="cellIs" dxfId="116" priority="114" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="116" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G61:P70">
-    <cfRule type="cellIs" dxfId="115" priority="113" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="115" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G62:P70">
-    <cfRule type="cellIs" dxfId="114" priority="112" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="114" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G71:P80">
-    <cfRule type="cellIs" dxfId="113" priority="111" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="113" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G81:P90">
-    <cfRule type="cellIs" dxfId="112" priority="110" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="112" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G82:P90">
-    <cfRule type="cellIs" dxfId="111" priority="109" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="111" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G91:P100">
-    <cfRule type="cellIs" dxfId="110" priority="108" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="110" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G101:P110">
-    <cfRule type="cellIs" dxfId="109" priority="107" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="109" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G102:P110">
-    <cfRule type="cellIs" dxfId="108" priority="106" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="108" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G111:P120">
-    <cfRule type="cellIs" dxfId="107" priority="105" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="107" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G121:P130">
-    <cfRule type="cellIs" dxfId="106" priority="104" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="106" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G122:P130">
-    <cfRule type="cellIs" dxfId="105" priority="103" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="105" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G131:P140">
-    <cfRule type="cellIs" dxfId="104" priority="102" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="104" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G141:P150">
-    <cfRule type="cellIs" dxfId="103" priority="101" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="103" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G142:P150">
-    <cfRule type="cellIs" dxfId="102" priority="100" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="102" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G151:P160">
-    <cfRule type="cellIs" dxfId="101" priority="99" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="101" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G161:P170">
-    <cfRule type="cellIs" dxfId="100" priority="98" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="100" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G162:P170">
-    <cfRule type="cellIs" dxfId="99" priority="97" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="99" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L180:P180 H171:P171 K172:P172 J173:P173 K174:P174 I175:P175 M176:P176 H177:P177 L178:P178 I179:P179">
-    <cfRule type="cellIs" dxfId="98" priority="96" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="98" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G187:P187 J181:P182 M183:P183 J184:P184 I185:P185 H186:P186 H190:P190 H188:P188 J189:P189">
-    <cfRule type="cellIs" dxfId="97" priority="95" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="97" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G187:P187 J182:P182 M183:P183 J184:P184 I185:P185 H186:P186 H190:P190 H188:P188 J189:P189">
-    <cfRule type="cellIs" dxfId="96" priority="94" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="96" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K191:P191 L192:P192 H193:P194 K195:P195 J196:P197 H198:P200">
-    <cfRule type="cellIs" dxfId="95" priority="93" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="95" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J210:P210 L201:P201 H202:P203 J204:P204 I205:P205 H206:P206 J207:P208 I209:P209">
-    <cfRule type="cellIs" dxfId="94" priority="92" operator="equal">
+  <conditionalFormatting sqref="J210:P210 L201:P201 H202:P202 J204:P204 I205:P205 H206:P206 J207:P208 I209:P209 I203:P203">
+    <cfRule type="cellIs" dxfId="93" priority="94" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J210:P210 H202:P203 J204:P204 I205:P205 H206:P206 J207:P208 I209:P209">
-    <cfRule type="cellIs" dxfId="93" priority="91" operator="equal">
+  <conditionalFormatting sqref="J210:P210 H202:P202 J204:P204 I205:P205 H206:P206 J207:P208 I209:P209 I203:P203">
+    <cfRule type="cellIs" dxfId="92" priority="93" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G215:P215 H211:P211 L212:P212 J213:P213 H214:P214 J216:P216 H217:P217 I218:P218 H219:P220">
-    <cfRule type="cellIs" dxfId="92" priority="90" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="92" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G221:P230">
-    <cfRule type="cellIs" dxfId="91" priority="89" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="91" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G222:P230">
-    <cfRule type="cellIs" dxfId="90" priority="88" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="90" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G231:P240">
-    <cfRule type="cellIs" dxfId="89" priority="87" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="89" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G241:P250">
-    <cfRule type="cellIs" dxfId="88" priority="86" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="88" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G242:P250">
-    <cfRule type="cellIs" dxfId="87" priority="85" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="87" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G251:P260">
-    <cfRule type="cellIs" dxfId="86" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="86" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G261:P270">
-    <cfRule type="cellIs" dxfId="85" priority="83" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="85" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G262:P270">
-    <cfRule type="cellIs" dxfId="84" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="84" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G271:P280">
-    <cfRule type="cellIs" dxfId="83" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="83" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G281:P290">
-    <cfRule type="cellIs" dxfId="82" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="82" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G282:P290">
-    <cfRule type="cellIs" dxfId="81" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="81" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G291:P300">
-    <cfRule type="cellIs" dxfId="80" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="80" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G301:P310">
-    <cfRule type="cellIs" dxfId="79" priority="77" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="79" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G302:P310">
-    <cfRule type="cellIs" dxfId="78" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="78" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G311:P320">
-    <cfRule type="cellIs" dxfId="77" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="77" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G321:P330">
-    <cfRule type="cellIs" dxfId="76" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="76" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G322:P330">
-    <cfRule type="cellIs" dxfId="75" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="75" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G331:P340">
-    <cfRule type="cellIs" dxfId="74" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="74" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G341:P350">
-    <cfRule type="cellIs" dxfId="73" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="73" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G342:P350">
-    <cfRule type="cellIs" dxfId="72" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="72" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G351:P360">
-    <cfRule type="cellIs" dxfId="71" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="71" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G361:P370">
-    <cfRule type="cellIs" dxfId="70" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="70" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G362:P370">
-    <cfRule type="cellIs" dxfId="69" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="69" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G371:P380">
-    <cfRule type="cellIs" dxfId="68" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="68" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G171">
-    <cfRule type="cellIs" dxfId="67" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="67" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G172:J172">
-    <cfRule type="cellIs" dxfId="66" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="66" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G173:I173">
-    <cfRule type="cellIs" dxfId="65" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="65" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G174:J174">
-    <cfRule type="cellIs" dxfId="64" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="64" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G175:H175">
-    <cfRule type="cellIs" dxfId="63" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="63" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G176:L176">
-    <cfRule type="cellIs" dxfId="62" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="62" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G177">
-    <cfRule type="cellIs" dxfId="61" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="61" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G178:K178">
-    <cfRule type="cellIs" dxfId="60" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="60" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G179:H179">
-    <cfRule type="cellIs" dxfId="59" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="59" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G180:K180">
-    <cfRule type="cellIs" dxfId="58" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="58" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G181:I181">
-    <cfRule type="cellIs" dxfId="57" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="57" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G181:I181">
-    <cfRule type="cellIs" dxfId="56" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="56" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G182:I182">
-    <cfRule type="cellIs" dxfId="55" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="55" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G182:I182">
-    <cfRule type="cellIs" dxfId="54" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="54" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G183:L183">
-    <cfRule type="cellIs" dxfId="53" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="53" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G183:L183">
-    <cfRule type="cellIs" dxfId="52" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="52" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G184:I184">
-    <cfRule type="cellIs" dxfId="51" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="51" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G184:I184">
-    <cfRule type="cellIs" dxfId="50" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="50" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G185:H185">
-    <cfRule type="cellIs" dxfId="49" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="49" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G185:H185">
-    <cfRule type="cellIs" dxfId="48" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="48" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G186">
-    <cfRule type="cellIs" dxfId="47" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="47" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G186">
-    <cfRule type="cellIs" dxfId="46" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="46" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G188">
-    <cfRule type="cellIs" dxfId="45" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="45" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G188">
-    <cfRule type="cellIs" dxfId="44" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="44" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G189:I189">
-    <cfRule type="cellIs" dxfId="43" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="43" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G189:I189">
-    <cfRule type="cellIs" dxfId="42" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="42" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G190">
-    <cfRule type="cellIs" dxfId="41" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="41" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G190">
-    <cfRule type="cellIs" dxfId="40" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="40" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G191:J191">
-    <cfRule type="cellIs" dxfId="39" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="39" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G192:K192">
-    <cfRule type="cellIs" dxfId="38" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="38" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G193:G194">
-    <cfRule type="cellIs" dxfId="37" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="37" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G195:J195">
-    <cfRule type="cellIs" dxfId="36" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="36" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G196:I196">
-    <cfRule type="cellIs" dxfId="35" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="35" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G197:I197">
-    <cfRule type="cellIs" dxfId="34" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="34" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G198">
-    <cfRule type="cellIs" dxfId="33" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="33" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G199:G200">
-    <cfRule type="cellIs" dxfId="32" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="32" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G201:K201">
-    <cfRule type="cellIs" dxfId="31" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="31" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G201:K201">
-    <cfRule type="cellIs" dxfId="30" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="30" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G202">
-    <cfRule type="cellIs" dxfId="29" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="29" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G202">
-    <cfRule type="cellIs" dxfId="28" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="28" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G203">
-    <cfRule type="cellIs" dxfId="27" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="27" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G203">
-    <cfRule type="cellIs" dxfId="26" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="26" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G204:I204">
-    <cfRule type="cellIs" dxfId="25" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="25" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G204:I204">
-    <cfRule type="cellIs" dxfId="24" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="24" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G205:H205">
-    <cfRule type="cellIs" dxfId="23" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="23" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G205:H205">
-    <cfRule type="cellIs" dxfId="22" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="22" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G206">
-    <cfRule type="cellIs" dxfId="21" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="21" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G206">
-    <cfRule type="cellIs" dxfId="20" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="20" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G207:I207">
-    <cfRule type="cellIs" dxfId="19" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="19" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G207:I207">
-    <cfRule type="cellIs" dxfId="18" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="18" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G208:I208">
-    <cfRule type="cellIs" dxfId="17" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G208:I208">
-    <cfRule type="cellIs" dxfId="16" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="16" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G209:H209">
-    <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="15" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G209:H209">
-    <cfRule type="cellIs" dxfId="14" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G210:I210">
-    <cfRule type="cellIs" dxfId="13" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="13" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G210:I210">
-    <cfRule type="cellIs" dxfId="12" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G211">
-    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G212:K212">
-    <cfRule type="cellIs" dxfId="10" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G213:I213">
-    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G214">
-    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G216:I216">
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G217">
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G218:H218">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G219">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G220">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>$J$4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H203">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>$J$4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H203">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>